<commit_message>
Added initial utlility demand as well as resulting initial operating costs and initial emissions
</commit_message>
<xml_diff>
--- a/data/Zweifel.xlsx
+++ b/data/Zweifel.xlsx
@@ -1943,7 +1943,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O20" sqref="O20"/>
+      <selection pane="bottomLeft" activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="F9" s="4">
         <f>K9/(G9*(D9-E9))</f>
-        <v>1.379E-2</v>
+        <v>2.5590909090909088E-4</v>
       </c>
       <c r="G9" s="2">
         <v>220000</v>
@@ -2326,7 +2326,7 @@
         <v>4410</v>
       </c>
       <c r="K9" s="5">
-        <v>3033.8</v>
+        <v>56.3</v>
       </c>
       <c r="L9" s="2">
         <v>0</v>
@@ -2708,7 +2708,7 @@
       </c>
       <c r="F18" s="4">
         <f>K18/(G18*(D18-E18))</f>
-        <v>1.2602727272727272E-2</v>
+        <v>2.095909090909091E-3</v>
       </c>
       <c r="G18" s="2">
         <v>220000</v>
@@ -2723,7 +2723,7 @@
         <v>7020</v>
       </c>
       <c r="K18" s="5">
-        <v>2772.6</v>
+        <v>461.1</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Updated case study data
</commit_message>
<xml_diff>
--- a/data/Zweifel.xlsx
+++ b/data/Zweifel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F849C18-793D-4750-A72F-6BC51CA80C14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02065ABF-F58B-4202-A30C-07F94E63114D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29880" yWindow="1395" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EAM" sheetId="1" r:id="rId1"/>
@@ -2887,6 +2887,9 @@
       <c r="C2">
         <v>10</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Moved read results from main to a new Jupyter notebook
</commit_message>
<xml_diff>
--- a/data/Zweifel.xlsx
+++ b/data/Zweifel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D214C6CC-BDD6-4463-B6D2-386C8B4C4100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8BC2B5-8F22-4774-A69A-7A0C0EC44F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23280" yWindow="3945" windowWidth="21600" windowHeight="12735" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EAM" sheetId="1" r:id="rId1"/>
@@ -242,6 +242,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -287,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -295,6 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -577,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
     </sheetView>
@@ -1953,13 +1957,13 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2348,7 +2352,8 @@
         <v>0.08</v>
       </c>
       <c r="O9" s="2">
-        <v>0.21</v>
+        <f>56.2/0.9/277777.78</f>
+        <v>2.2479999820159999E-4</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2395,8 +2400,9 @@
       <c r="N10" s="1">
         <v>0.04</v>
       </c>
-      <c r="O10" s="1">
-        <v>0.21</v>
+      <c r="O10" s="7">
+        <f>0.000128/(0.55*(273.15-5 )/25)</f>
+        <v>2.1697489532656418E-5</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2745,7 +2751,8 @@
         <v>0.08</v>
       </c>
       <c r="O18" s="2">
-        <v>0.21</v>
+        <f>56.2/0.9/277777.78</f>
+        <v>2.2479999820159999E-4</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2792,8 +2799,9 @@
       <c r="N19" s="1">
         <v>0.04</v>
       </c>
-      <c r="O19" s="1">
-        <v>0.21</v>
+      <c r="O19" s="7">
+        <f>0.000128/(0.55*(273.15-5 )/25)</f>
+        <v>2.1697489532656418E-5</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -2852,7 +2860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>

</xml_diff>